<commit_message>
Update sprint burn down
</commit_message>
<xml_diff>
--- a/SprintBurnDown.xlsx
+++ b/SprintBurnDown.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chung1991/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chung1991/Desktop/WebEnterprise/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1097,13 +1097,13 @@
                   <c:v>155.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>155.0</c:v>
+                  <c:v>105.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>155.0</c:v>
+                  <c:v>105.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>155.0</c:v>
+                  <c:v>105.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1157,11 +1157,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-2134380544"/>
-        <c:axId val="-2105502048"/>
+        <c:axId val="-2024906368"/>
+        <c:axId val="-2052717664"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2134380544"/>
+        <c:axId val="-2024906368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1200,7 +1200,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2105502048"/>
+        <c:crossAx val="-2052717664"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1208,7 +1208,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2105502048"/>
+        <c:axId val="-2052717664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1252,7 +1252,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2134380544"/>
+        <c:crossAx val="-2024906368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1409,61 +1409,61 @@
                   <c:v>155.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>155.0</c:v>
+                  <c:v>105.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>155.0</c:v>
+                  <c:v>105.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>155.0</c:v>
+                  <c:v>105.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>155.0</c:v>
+                  <c:v>105.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>155.0</c:v>
+                  <c:v>105.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>155.0</c:v>
+                  <c:v>105.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>155.0</c:v>
+                  <c:v>105.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>155.0</c:v>
+                  <c:v>105.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>155.0</c:v>
+                  <c:v>105.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>155.0</c:v>
+                  <c:v>105.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>155.0</c:v>
+                  <c:v>105.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>155.0</c:v>
+                  <c:v>105.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>155.0</c:v>
+                  <c:v>105.0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>155.0</c:v>
+                  <c:v>105.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>155.0</c:v>
+                  <c:v>105.0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>155.0</c:v>
+                  <c:v>105.0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>155.0</c:v>
+                  <c:v>105.0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>155.0</c:v>
+                  <c:v>105.0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>155.0</c:v>
+                  <c:v>105.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1565,11 +1565,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-2133922176"/>
-        <c:axId val="-2136464592"/>
+        <c:axId val="-2053061648"/>
+        <c:axId val="-2052741280"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2133922176"/>
+        <c:axId val="-2053061648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1591,7 +1591,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -1608,7 +1607,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2136464592"/>
+        <c:crossAx val="-2052741280"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1616,7 +1615,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2136464592"/>
+        <c:axId val="-2052741280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1638,7 +1637,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -1660,14 +1658,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2133922176"/>
+        <c:crossAx val="-2053061648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2020,10 +2017,10 @@
   <dimension ref="A1:BM101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="X36" sqref="X36"/>
+      <selection pane="bottomRight" activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2392,11 +2389,13 @@
       </c>
       <c r="D4" s="8">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="E4" s="15"/>
       <c r="F4" s="16"/>
-      <c r="G4" s="16"/>
+      <c r="G4" s="16">
+        <v>30</v>
+      </c>
       <c r="BM4" s="17"/>
     </row>
     <row r="5" spans="1:65" ht="26" x14ac:dyDescent="0.15">
@@ -2472,11 +2471,14 @@
       </c>
       <c r="D8" s="8">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="E8" s="15"/>
       <c r="F8">
         <v>110</v>
+      </c>
+      <c r="G8">
+        <v>20</v>
       </c>
       <c r="K8" s="16"/>
       <c r="L8" s="16"/>
@@ -2963,7 +2965,7 @@
       </c>
       <c r="D35" s="27">
         <f t="shared" si="2"/>
-        <v>155</v>
+        <v>105</v>
       </c>
       <c r="E35" s="28">
         <f t="shared" ref="E35:BM35" si="3">SUM(E3:E19)</f>
@@ -2975,7 +2977,7 @@
       </c>
       <c r="G35" s="28">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="H35" s="28">
         <f t="shared" si="3"/>
@@ -3603,239 +3605,239 @@
       </c>
       <c r="G38" s="40">
         <f t="shared" si="5"/>
-        <v>155</v>
+        <v>105</v>
       </c>
       <c r="H38" s="40">
         <f t="shared" si="5"/>
-        <v>155</v>
+        <v>105</v>
       </c>
       <c r="I38" s="40">
         <f t="shared" si="5"/>
-        <v>155</v>
+        <v>105</v>
       </c>
       <c r="J38" s="40">
         <f t="shared" si="5"/>
-        <v>155</v>
+        <v>105</v>
       </c>
       <c r="K38" s="40">
         <f t="shared" si="5"/>
-        <v>155</v>
+        <v>105</v>
       </c>
       <c r="L38" s="40">
         <f t="shared" si="5"/>
-        <v>155</v>
+        <v>105</v>
       </c>
       <c r="M38" s="40">
         <f t="shared" si="5"/>
-        <v>155</v>
+        <v>105</v>
       </c>
       <c r="N38" s="40">
         <f t="shared" si="5"/>
-        <v>155</v>
+        <v>105</v>
       </c>
       <c r="O38" s="40">
         <f t="shared" si="5"/>
-        <v>155</v>
+        <v>105</v>
       </c>
       <c r="P38" s="40">
         <f t="shared" si="5"/>
-        <v>155</v>
+        <v>105</v>
       </c>
       <c r="Q38" s="40">
         <f t="shared" si="5"/>
-        <v>155</v>
+        <v>105</v>
       </c>
       <c r="R38" s="40">
         <f t="shared" si="5"/>
-        <v>155</v>
+        <v>105</v>
       </c>
       <c r="S38" s="40">
         <f t="shared" si="5"/>
-        <v>155</v>
+        <v>105</v>
       </c>
       <c r="T38" s="40">
         <f t="shared" si="5"/>
-        <v>155</v>
+        <v>105</v>
       </c>
       <c r="U38" s="40">
         <f t="shared" si="5"/>
-        <v>155</v>
+        <v>105</v>
       </c>
       <c r="V38" s="40">
         <f t="shared" si="5"/>
-        <v>155</v>
+        <v>105</v>
       </c>
       <c r="W38" s="40">
         <f t="shared" si="5"/>
-        <v>155</v>
+        <v>105</v>
       </c>
       <c r="X38" s="38">
         <f t="shared" si="5"/>
-        <v>155</v>
+        <v>105</v>
       </c>
       <c r="Y38" s="38">
         <f t="shared" si="5"/>
-        <v>155</v>
+        <v>105</v>
       </c>
       <c r="Z38" s="38">
         <f t="shared" si="5"/>
-        <v>155</v>
+        <v>105</v>
       </c>
       <c r="AA38" s="38">
         <f t="shared" si="5"/>
-        <v>155</v>
+        <v>105</v>
       </c>
       <c r="AB38" s="38">
         <f t="shared" si="5"/>
-        <v>155</v>
+        <v>105</v>
       </c>
       <c r="AC38" s="38">
         <f t="shared" si="5"/>
-        <v>155</v>
+        <v>105</v>
       </c>
       <c r="AD38" s="38">
         <f t="shared" si="5"/>
-        <v>155</v>
+        <v>105</v>
       </c>
       <c r="AE38" s="38">
         <f t="shared" si="5"/>
-        <v>155</v>
+        <v>105</v>
       </c>
       <c r="AF38" s="38">
         <f t="shared" si="5"/>
-        <v>155</v>
+        <v>105</v>
       </c>
       <c r="AG38" s="38">
         <f t="shared" si="5"/>
-        <v>155</v>
+        <v>105</v>
       </c>
       <c r="AH38" s="38">
         <f t="shared" si="5"/>
-        <v>155</v>
+        <v>105</v>
       </c>
       <c r="AI38" s="38">
         <f t="shared" si="5"/>
-        <v>155</v>
+        <v>105</v>
       </c>
       <c r="AJ38" s="38">
         <f t="shared" si="5"/>
-        <v>155</v>
+        <v>105</v>
       </c>
       <c r="AK38" s="38">
         <f t="shared" si="5"/>
-        <v>155</v>
+        <v>105</v>
       </c>
       <c r="AL38" s="38">
         <f t="shared" si="5"/>
-        <v>155</v>
+        <v>105</v>
       </c>
       <c r="AM38" s="38">
         <f t="shared" si="5"/>
-        <v>155</v>
+        <v>105</v>
       </c>
       <c r="AN38" s="38">
         <f t="shared" si="5"/>
-        <v>155</v>
+        <v>105</v>
       </c>
       <c r="AO38" s="38">
         <f t="shared" si="5"/>
-        <v>155</v>
+        <v>105</v>
       </c>
       <c r="AP38" s="38">
         <f t="shared" si="5"/>
-        <v>155</v>
+        <v>105</v>
       </c>
       <c r="AQ38" s="38">
         <f t="shared" si="5"/>
-        <v>155</v>
+        <v>105</v>
       </c>
       <c r="AR38" s="38">
         <f t="shared" si="5"/>
-        <v>155</v>
+        <v>105</v>
       </c>
       <c r="AS38" s="38">
         <f t="shared" si="5"/>
-        <v>155</v>
+        <v>105</v>
       </c>
       <c r="AT38" s="38">
         <f t="shared" si="5"/>
-        <v>155</v>
+        <v>105</v>
       </c>
       <c r="AU38" s="38">
         <f t="shared" si="5"/>
-        <v>155</v>
+        <v>105</v>
       </c>
       <c r="AV38" s="38">
         <f t="shared" si="5"/>
-        <v>155</v>
+        <v>105</v>
       </c>
       <c r="AW38" s="38">
         <f t="shared" si="5"/>
-        <v>155</v>
+        <v>105</v>
       </c>
       <c r="AX38" s="38">
         <f t="shared" si="5"/>
-        <v>155</v>
+        <v>105</v>
       </c>
       <c r="AY38" s="38">
         <f t="shared" si="5"/>
-        <v>155</v>
+        <v>105</v>
       </c>
       <c r="AZ38" s="38">
         <f t="shared" si="5"/>
-        <v>155</v>
+        <v>105</v>
       </c>
       <c r="BA38" s="38">
         <f t="shared" si="5"/>
-        <v>155</v>
+        <v>105</v>
       </c>
       <c r="BB38" s="38">
         <f t="shared" si="5"/>
-        <v>155</v>
+        <v>105</v>
       </c>
       <c r="BC38" s="38">
         <f t="shared" si="5"/>
-        <v>155</v>
+        <v>105</v>
       </c>
       <c r="BD38" s="38">
         <f t="shared" si="5"/>
-        <v>155</v>
+        <v>105</v>
       </c>
       <c r="BE38" s="38">
         <f t="shared" si="5"/>
-        <v>155</v>
+        <v>105</v>
       </c>
       <c r="BF38" s="38">
         <f t="shared" si="5"/>
-        <v>155</v>
+        <v>105</v>
       </c>
       <c r="BG38" s="38">
         <f t="shared" si="5"/>
-        <v>155</v>
+        <v>105</v>
       </c>
       <c r="BH38" s="38">
         <f t="shared" si="5"/>
-        <v>155</v>
+        <v>105</v>
       </c>
       <c r="BI38" s="38">
         <f t="shared" si="5"/>
-        <v>155</v>
+        <v>105</v>
       </c>
       <c r="BJ38" s="38">
         <f t="shared" si="5"/>
-        <v>155</v>
+        <v>105</v>
       </c>
       <c r="BK38" s="38">
         <f t="shared" si="5"/>
-        <v>155</v>
+        <v>105</v>
       </c>
       <c r="BL38" s="38">
         <f t="shared" si="5"/>
-        <v>155</v>
+        <v>105</v>
       </c>
       <c r="BM38" s="38">
         <f t="shared" si="5"/>
-        <v>155</v>
+        <v>105</v>
       </c>
     </row>
     <row r="39" spans="1:65" ht="18" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
SQL Injection execiser Update Sprint burn down
</commit_message>
<xml_diff>
--- a/SprintBurnDown.xlsx
+++ b/SprintBurnDown.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25420" windowHeight="14680"/>
+    <workbookView xWindow="1820" yWindow="460" windowWidth="23600" windowHeight="14680"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint 4" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="42">
   <si>
     <t>Task</t>
   </si>
@@ -133,6 +133,24 @@
   </si>
   <si>
     <t>Edit v2.sql &amp; Create tracking excel</t>
+  </si>
+  <si>
+    <t>Research Linux Security Example</t>
+  </si>
+  <si>
+    <t>Research meaningful course report information</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CL take Annual Course </t>
+  </si>
+  <si>
+    <t>Design responsive table</t>
+  </si>
+  <si>
+    <t>Create layout for main page of admin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DLT/PVC can view CMR </t>
   </si>
 </sst>
 </file>
@@ -1013,19 +1031,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="22"/>
                 <c:pt idx="0">
-                  <c:v>290.0</c:v>
+                  <c:v>510.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>232.0</c:v>
+                  <c:v>408.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>174.0</c:v>
+                  <c:v>306.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>116.0</c:v>
+                  <c:v>204.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>58.0</c:v>
+                  <c:v>102.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0.0</c:v>
@@ -1088,22 +1106,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>290.0</c:v>
+                  <c:v>510.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>270.0</c:v>
+                  <c:v>490.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>155.0</c:v>
+                  <c:v>375.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>105.0</c:v>
+                  <c:v>325.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>105.0</c:v>
+                  <c:v>285.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>105.0</c:v>
+                  <c:v>285.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1126,19 +1144,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>290.0</c:v>
+                  <c:v>510.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>232.0</c:v>
+                  <c:v>408.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>174.0</c:v>
+                  <c:v>306.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>116.0</c:v>
+                  <c:v>204.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>58.0</c:v>
+                  <c:v>102.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0.0</c:v>
@@ -1157,11 +1175,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-2024906368"/>
-        <c:axId val="-2052717664"/>
+        <c:axId val="-2111714592"/>
+        <c:axId val="-2110554960"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2024906368"/>
+        <c:axId val="-2111714592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1200,7 +1218,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2052717664"/>
+        <c:crossAx val="-2110554960"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1208,7 +1226,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2052717664"/>
+        <c:axId val="-2110554960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1252,7 +1270,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2024906368"/>
+        <c:crossAx val="-2111714592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1325,19 +1343,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="22"/>
                 <c:pt idx="0">
-                  <c:v>290.0</c:v>
+                  <c:v>510.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>232.0</c:v>
+                  <c:v>408.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>174.0</c:v>
+                  <c:v>306.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>116.0</c:v>
+                  <c:v>204.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>58.0</c:v>
+                  <c:v>102.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0.0</c:v>
@@ -1400,70 +1418,70 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="22"/>
                 <c:pt idx="0">
-                  <c:v>290.0</c:v>
+                  <c:v>510.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>270.0</c:v>
+                  <c:v>490.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>155.0</c:v>
+                  <c:v>375.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>105.0</c:v>
+                  <c:v>325.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>105.0</c:v>
+                  <c:v>285.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>105.0</c:v>
+                  <c:v>285.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>105.0</c:v>
+                  <c:v>285.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>105.0</c:v>
+                  <c:v>285.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>105.0</c:v>
+                  <c:v>285.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>105.0</c:v>
+                  <c:v>285.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>105.0</c:v>
+                  <c:v>285.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>105.0</c:v>
+                  <c:v>285.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>105.0</c:v>
+                  <c:v>285.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>105.0</c:v>
+                  <c:v>285.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>105.0</c:v>
+                  <c:v>285.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>105.0</c:v>
+                  <c:v>285.0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>105.0</c:v>
+                  <c:v>285.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>105.0</c:v>
+                  <c:v>285.0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>105.0</c:v>
+                  <c:v>285.0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>105.0</c:v>
+                  <c:v>285.0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>105.0</c:v>
+                  <c:v>285.0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>105.0</c:v>
+                  <c:v>285.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1486,19 +1504,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="22"/>
                 <c:pt idx="0">
-                  <c:v>290.0</c:v>
+                  <c:v>510.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>232.0</c:v>
+                  <c:v>408.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>174.0</c:v>
+                  <c:v>306.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>116.0</c:v>
+                  <c:v>204.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>58.0</c:v>
+                  <c:v>102.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0.0</c:v>
@@ -1565,11 +1583,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-2053061648"/>
-        <c:axId val="-2052741280"/>
+        <c:axId val="-2111689040"/>
+        <c:axId val="-2111683856"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2053061648"/>
+        <c:axId val="-2111689040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1607,7 +1625,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2052741280"/>
+        <c:crossAx val="-2111683856"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1615,7 +1633,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2052741280"/>
+        <c:axId val="-2111683856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1658,7 +1676,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2053061648"/>
+        <c:crossAx val="-2111689040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2017,10 +2035,10 @@
   <dimension ref="A1:BM101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G9" sqref="G9"/>
+      <selection pane="bottomRight" activeCell="I37" sqref="I37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2551,47 +2569,62 @@
       <c r="P11" s="16"/>
       <c r="BM11" s="17"/>
     </row>
-    <row r="12" spans="1:65" ht="13" x14ac:dyDescent="0.15">
-      <c r="A12" s="13"/>
-      <c r="B12" s="14"/>
+    <row r="12" spans="1:65" ht="26" x14ac:dyDescent="0.15">
+      <c r="A12" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" s="14">
+        <v>80</v>
+      </c>
       <c r="C12" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="D12" s="8">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="E12" s="15"/>
+      <c r="H12">
+        <v>40</v>
+      </c>
       <c r="P12" s="16"/>
       <c r="Q12" s="16"/>
       <c r="BM12" s="17"/>
     </row>
-    <row r="13" spans="1:65" ht="13" x14ac:dyDescent="0.15">
-      <c r="A13" s="13"/>
-      <c r="B13" s="14"/>
+    <row r="13" spans="1:65" ht="26" x14ac:dyDescent="0.15">
+      <c r="A13" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" s="14">
+        <v>40</v>
+      </c>
       <c r="C13" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="D13" s="8">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="E13" s="15"/>
       <c r="Q13" s="16"/>
       <c r="BM13" s="17"/>
     </row>
     <row r="14" spans="1:65" ht="13" x14ac:dyDescent="0.15">
-      <c r="A14" s="13"/>
-      <c r="B14" s="14"/>
+      <c r="A14" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" s="14">
+        <v>30</v>
+      </c>
       <c r="C14" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="D14" s="8">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="E14" s="15"/>
       <c r="R14" s="16"/>
@@ -2599,15 +2632,19 @@
       <c r="BM14" s="17"/>
     </row>
     <row r="15" spans="1:65" ht="13" x14ac:dyDescent="0.15">
-      <c r="A15" s="13"/>
-      <c r="B15" s="14"/>
+      <c r="A15" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" s="14">
+        <v>20</v>
+      </c>
       <c r="C15" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="D15" s="8">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="E15" s="15"/>
       <c r="R15" s="16"/>
@@ -2616,16 +2653,20 @@
       <c r="U15" s="16"/>
       <c r="BM15" s="17"/>
     </row>
-    <row r="16" spans="1:65" ht="13" x14ac:dyDescent="0.15">
-      <c r="A16" s="13"/>
-      <c r="B16" s="14"/>
+    <row r="16" spans="1:65" ht="26" x14ac:dyDescent="0.15">
+      <c r="A16" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" s="14">
+        <v>20</v>
+      </c>
       <c r="C16" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="D16" s="8">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="E16" s="15"/>
       <c r="R16" s="16"/>
@@ -2636,15 +2677,19 @@
       <c r="BM16" s="17"/>
     </row>
     <row r="17" spans="1:65" ht="13" x14ac:dyDescent="0.15">
-      <c r="A17" s="13"/>
-      <c r="B17" s="14"/>
+      <c r="A17" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" s="14">
+        <v>30</v>
+      </c>
       <c r="C17" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="D17" s="8">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="E17" s="15"/>
       <c r="V17" s="16"/>
@@ -2957,15 +3002,15 @@
       </c>
       <c r="B35" s="26">
         <f t="shared" ref="B35:D35" si="2">SUM(B3:B34)</f>
-        <v>290</v>
+        <v>510</v>
       </c>
       <c r="C35" s="27">
         <f t="shared" si="2"/>
-        <v>290</v>
+        <v>510</v>
       </c>
       <c r="D35" s="27">
         <f t="shared" si="2"/>
-        <v>105</v>
+        <v>285</v>
       </c>
       <c r="E35" s="28">
         <f t="shared" ref="E35:BM35" si="3">SUM(E3:E19)</f>
@@ -2981,7 +3026,7 @@
       </c>
       <c r="H35" s="28">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="I35" s="28">
         <f t="shared" si="3"/>
@@ -3223,19 +3268,19 @@
       <c r="C36" s="31"/>
       <c r="D36" s="32"/>
       <c r="E36" s="33">
-        <v>58</v>
+        <v>102</v>
       </c>
       <c r="F36" s="34">
-        <v>58</v>
+        <v>102</v>
       </c>
       <c r="G36" s="34">
-        <v>58</v>
+        <v>102</v>
       </c>
       <c r="H36" s="34">
-        <v>58</v>
+        <v>102</v>
       </c>
       <c r="I36" s="34">
-        <v>58</v>
+        <v>102</v>
       </c>
       <c r="J36" s="34">
         <v>0</v>
@@ -3336,23 +3381,23 @@
       </c>
       <c r="D37" s="40">
         <f>B35</f>
-        <v>290</v>
+        <v>510</v>
       </c>
       <c r="E37" s="41">
         <f t="shared" ref="E37:BM37" si="4">D37-E36</f>
-        <v>232</v>
+        <v>408</v>
       </c>
       <c r="F37" s="41">
         <f t="shared" si="4"/>
-        <v>174</v>
+        <v>306</v>
       </c>
       <c r="G37" s="41">
         <f t="shared" si="4"/>
-        <v>116</v>
+        <v>204</v>
       </c>
       <c r="H37" s="41">
         <f t="shared" si="4"/>
-        <v>58</v>
+        <v>102</v>
       </c>
       <c r="I37" s="41">
         <f t="shared" si="4"/>
@@ -3593,251 +3638,251 @@
       </c>
       <c r="D38" s="40">
         <f>C35</f>
-        <v>290</v>
+        <v>510</v>
       </c>
       <c r="E38" s="40">
         <f>$C$35-SUM(E$3:E$34)</f>
-        <v>270</v>
+        <v>490</v>
       </c>
       <c r="F38" s="40">
         <f t="shared" ref="F38:BM38" si="5">E38-SUM(F3:F34)</f>
-        <v>155</v>
+        <v>375</v>
       </c>
       <c r="G38" s="40">
         <f t="shared" si="5"/>
-        <v>105</v>
+        <v>325</v>
       </c>
       <c r="H38" s="40">
         <f t="shared" si="5"/>
-        <v>105</v>
+        <v>285</v>
       </c>
       <c r="I38" s="40">
         <f t="shared" si="5"/>
-        <v>105</v>
+        <v>285</v>
       </c>
       <c r="J38" s="40">
         <f t="shared" si="5"/>
-        <v>105</v>
+        <v>285</v>
       </c>
       <c r="K38" s="40">
         <f t="shared" si="5"/>
-        <v>105</v>
+        <v>285</v>
       </c>
       <c r="L38" s="40">
         <f t="shared" si="5"/>
-        <v>105</v>
+        <v>285</v>
       </c>
       <c r="M38" s="40">
         <f t="shared" si="5"/>
-        <v>105</v>
+        <v>285</v>
       </c>
       <c r="N38" s="40">
         <f t="shared" si="5"/>
-        <v>105</v>
+        <v>285</v>
       </c>
       <c r="O38" s="40">
         <f t="shared" si="5"/>
-        <v>105</v>
+        <v>285</v>
       </c>
       <c r="P38" s="40">
         <f t="shared" si="5"/>
-        <v>105</v>
+        <v>285</v>
       </c>
       <c r="Q38" s="40">
         <f t="shared" si="5"/>
-        <v>105</v>
+        <v>285</v>
       </c>
       <c r="R38" s="40">
         <f t="shared" si="5"/>
-        <v>105</v>
+        <v>285</v>
       </c>
       <c r="S38" s="40">
         <f t="shared" si="5"/>
-        <v>105</v>
+        <v>285</v>
       </c>
       <c r="T38" s="40">
         <f t="shared" si="5"/>
-        <v>105</v>
+        <v>285</v>
       </c>
       <c r="U38" s="40">
         <f t="shared" si="5"/>
-        <v>105</v>
+        <v>285</v>
       </c>
       <c r="V38" s="40">
         <f t="shared" si="5"/>
-        <v>105</v>
+        <v>285</v>
       </c>
       <c r="W38" s="40">
         <f t="shared" si="5"/>
-        <v>105</v>
+        <v>285</v>
       </c>
       <c r="X38" s="38">
         <f t="shared" si="5"/>
-        <v>105</v>
+        <v>285</v>
       </c>
       <c r="Y38" s="38">
         <f t="shared" si="5"/>
-        <v>105</v>
+        <v>285</v>
       </c>
       <c r="Z38" s="38">
         <f t="shared" si="5"/>
-        <v>105</v>
+        <v>285</v>
       </c>
       <c r="AA38" s="38">
         <f t="shared" si="5"/>
-        <v>105</v>
+        <v>285</v>
       </c>
       <c r="AB38" s="38">
         <f t="shared" si="5"/>
-        <v>105</v>
+        <v>285</v>
       </c>
       <c r="AC38" s="38">
         <f t="shared" si="5"/>
-        <v>105</v>
+        <v>285</v>
       </c>
       <c r="AD38" s="38">
         <f t="shared" si="5"/>
-        <v>105</v>
+        <v>285</v>
       </c>
       <c r="AE38" s="38">
         <f t="shared" si="5"/>
-        <v>105</v>
+        <v>285</v>
       </c>
       <c r="AF38" s="38">
         <f t="shared" si="5"/>
-        <v>105</v>
+        <v>285</v>
       </c>
       <c r="AG38" s="38">
         <f t="shared" si="5"/>
-        <v>105</v>
+        <v>285</v>
       </c>
       <c r="AH38" s="38">
         <f t="shared" si="5"/>
-        <v>105</v>
+        <v>285</v>
       </c>
       <c r="AI38" s="38">
         <f t="shared" si="5"/>
-        <v>105</v>
+        <v>285</v>
       </c>
       <c r="AJ38" s="38">
         <f t="shared" si="5"/>
-        <v>105</v>
+        <v>285</v>
       </c>
       <c r="AK38" s="38">
         <f t="shared" si="5"/>
-        <v>105</v>
+        <v>285</v>
       </c>
       <c r="AL38" s="38">
         <f t="shared" si="5"/>
-        <v>105</v>
+        <v>285</v>
       </c>
       <c r="AM38" s="38">
         <f t="shared" si="5"/>
-        <v>105</v>
+        <v>285</v>
       </c>
       <c r="AN38" s="38">
         <f t="shared" si="5"/>
-        <v>105</v>
+        <v>285</v>
       </c>
       <c r="AO38" s="38">
         <f t="shared" si="5"/>
-        <v>105</v>
+        <v>285</v>
       </c>
       <c r="AP38" s="38">
         <f t="shared" si="5"/>
-        <v>105</v>
+        <v>285</v>
       </c>
       <c r="AQ38" s="38">
         <f t="shared" si="5"/>
-        <v>105</v>
+        <v>285</v>
       </c>
       <c r="AR38" s="38">
         <f t="shared" si="5"/>
-        <v>105</v>
+        <v>285</v>
       </c>
       <c r="AS38" s="38">
         <f t="shared" si="5"/>
-        <v>105</v>
+        <v>285</v>
       </c>
       <c r="AT38" s="38">
         <f t="shared" si="5"/>
-        <v>105</v>
+        <v>285</v>
       </c>
       <c r="AU38" s="38">
         <f t="shared" si="5"/>
-        <v>105</v>
+        <v>285</v>
       </c>
       <c r="AV38" s="38">
         <f t="shared" si="5"/>
-        <v>105</v>
+        <v>285</v>
       </c>
       <c r="AW38" s="38">
         <f t="shared" si="5"/>
-        <v>105</v>
+        <v>285</v>
       </c>
       <c r="AX38" s="38">
         <f t="shared" si="5"/>
-        <v>105</v>
+        <v>285</v>
       </c>
       <c r="AY38" s="38">
         <f t="shared" si="5"/>
-        <v>105</v>
+        <v>285</v>
       </c>
       <c r="AZ38" s="38">
         <f t="shared" si="5"/>
-        <v>105</v>
+        <v>285</v>
       </c>
       <c r="BA38" s="38">
         <f t="shared" si="5"/>
-        <v>105</v>
+        <v>285</v>
       </c>
       <c r="BB38" s="38">
         <f t="shared" si="5"/>
-        <v>105</v>
+        <v>285</v>
       </c>
       <c r="BC38" s="38">
         <f t="shared" si="5"/>
-        <v>105</v>
+        <v>285</v>
       </c>
       <c r="BD38" s="38">
         <f t="shared" si="5"/>
-        <v>105</v>
+        <v>285</v>
       </c>
       <c r="BE38" s="38">
         <f t="shared" si="5"/>
-        <v>105</v>
+        <v>285</v>
       </c>
       <c r="BF38" s="38">
         <f t="shared" si="5"/>
-        <v>105</v>
+        <v>285</v>
       </c>
       <c r="BG38" s="38">
         <f t="shared" si="5"/>
-        <v>105</v>
+        <v>285</v>
       </c>
       <c r="BH38" s="38">
         <f t="shared" si="5"/>
-        <v>105</v>
+        <v>285</v>
       </c>
       <c r="BI38" s="38">
         <f t="shared" si="5"/>
-        <v>105</v>
+        <v>285</v>
       </c>
       <c r="BJ38" s="38">
         <f t="shared" si="5"/>
-        <v>105</v>
+        <v>285</v>
       </c>
       <c r="BK38" s="38">
         <f t="shared" si="5"/>
-        <v>105</v>
+        <v>285</v>
       </c>
       <c r="BL38" s="38">
         <f t="shared" si="5"/>
-        <v>105</v>
+        <v>285</v>
       </c>
       <c r="BM38" s="38">
         <f t="shared" si="5"/>
-        <v>105</v>
+        <v>285</v>
       </c>
     </row>
     <row r="39" spans="1:65" ht="18" x14ac:dyDescent="0.2">

</xml_diff>